<commit_message>
Event Summary first draft
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
+++ b/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
@@ -557,7 +557,7 @@
   <si>
     <t>One would expect this element to be a cardinality  of 1..1.  The only circumstance in which the subject can be missing is when the observation is made by a device that does not know the patient. In this case, the observation SHALL be matched to a patient through some context/channel matching technique, and at this point, the observation should be updated. -If the target of the observation is different than the subject, the general extension [observation-focal-subject](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
+If the target of the observation is different than the subject, the general extension [observation-focal-subject](extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
@@ -713,7 +713,7 @@
     <t>Normally, an observation will have either a single value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and related observations (for an Apgar score, the observations from which the measure is derived). If a value is present, the datatype for this element should be determined by Observation.code. This element has a variable name depending on the type as follows: valueQuantity, valueCodeableConcept, valueString, valueBoolean, valueRange, valueRatio, valueSampledData, valueAttachment, valueTime, valueDateTime, or valuePeriod. (The name format is "'value' + the type name" with a capital on the first letter of the type).  -If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
+If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](observation.html#notes) below.</t>
   </si>
   <si>
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
@@ -840,7 +840,7 @@
     <t>Indicates the site on the subject's body where the observation was made (i.e. the target site).</t>
   </si>
   <si>
-    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-body-site-instance.html).</t>
+    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](extension-body-site-instance.html).</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1139,7 +1139,7 @@
     <t>A  reference to another resource (usually another Observation) whose relationship is defined by the relationship type code.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#4.20.4).</t>
+    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](observation.html#4.20.4).</t>
   </si>
   <si>
     <t>Normally, an observation will have either a value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and a set of related observations or sometimes a QuestionnaireResponse from which the measure is derived.</t>
@@ -1198,7 +1198,7 @@
     <t>Resource that is related to this one</t>
   </si>
   <si>
-    <t>A reference to the observation or [QuestionnaireResponse](https://build.fhir.org/ig/hl7au/au-fhir-base/questionnaireresponse.html#) resource that is related to this observation.</t>
+    <t>A reference to the observation or [QuestionnaireResponse](questionnaireresponse.html#) resource that is related to this observation.</t>
   </si>
   <si>
     <t>.targetObservation</t>
@@ -1213,7 +1213,7 @@
     <t>Some observations have multiple component observations.  These component observations are expressed as separate code value pairs that share the same attributes.  Examples include systolic and diastolic component observations for blood pressure measurement and multiple component observations for genetics observations.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
+    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](observation.html#notes) below.</t>
   </si>
   <si>
     <t>Component observations share the same attributes in the Observation resource as the primary observation and are always treated a part of a single observation (they are not separable).   However, the reference range for the primary observation value is not inherited by the component values and is required when appropriate for each component observation.</t>

</xml_diff>

<commit_message>
add shs build output
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
+++ b/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
@@ -557,7 +557,7 @@
   <si>
     <t>One would expect this element to be a cardinality  of 1..1.  The only circumstance in which the subject can be missing is when the observation is made by a device that does not know the patient. In this case, the observation SHALL be matched to a patient through some context/channel matching technique, and at this point, the observation should be updated. -If the target of the observation is different than the subject, the general extension [observation-focal-subject](http://hl7.org/fhir/STU3/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
+If the target of the observation is different than the subject, the general extension [observation-focal-subject](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
@@ -713,7 +713,7 @@
     <t>Normally, an observation will have either a single value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and related observations (for an Apgar score, the observations from which the measure is derived). If a value is present, the datatype for this element should be determined by Observation.code. This element has a variable name depending on the type as follows: valueQuantity, valueCodeableConcept, valueString, valueBoolean, valueRange, valueRatio, valueSampledData, valueAttachment, valueTime, valueDateTime, or valuePeriod. (The name format is "'value' + the type name" with a capital on the first letter of the type).  -If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
@@ -840,7 +840,7 @@
     <t>Indicates the site on the subject's body where the observation was made (i.e. the target site).</t>
   </si>
   <si>
-    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](http://hl7.org/fhir/STU3/extension-body-site-instance.html).</t>
+    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-body-site-instance.html).</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1139,7 +1139,7 @@
     <t>A  reference to another resource (usually another Observation) whose relationship is defined by the relationship type code.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](http://hl7.org/fhir/STU3/observation.html#4.20.4).</t>
+    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#4.20.4).</t>
   </si>
   <si>
     <t>Normally, an observation will have either a value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and a set of related observations or sometimes a QuestionnaireResponse from which the measure is derived.</t>
@@ -1198,7 +1198,7 @@
     <t>Resource that is related to this one</t>
   </si>
   <si>
-    <t>A reference to the observation or [QuestionnaireResponse](http://hl7.org/fhir/STU3/questionnaireresponse.html#) resource that is related to this observation.</t>
+    <t>A reference to the observation or [QuestionnaireResponse](https://build.fhir.org/ig/hl7au/au-fhir-base/questionnaireresponse.html#) resource that is related to this observation.</t>
   </si>
   <si>
     <t>.targetObservation</t>
@@ -1213,7 +1213,7 @@
     <t>Some observations have multiple component observations.  These component observations are expressed as separate code value pairs that share the same attributes.  Examples include systolic and diastolic component observations for blood pressure measurement and multiple component observations for genetics observations.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>Component observations share the same attributes in the Observation resource as the primary observation and are always treated a part of a single observation (they are not separable).   However, the reference range for the primary observation value is not inherited by the component values and is required when appropriate for each component observation.</t>

</xml_diff>

<commit_message>
De-containing SHS example 2
De-containing SHS example 2 ie first part of CIFMM-2306 and github "Fixes #9"
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
+++ b/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
@@ -557,7 +557,7 @@
   <si>
     <t>One would expect this element to be a cardinality  of 1..1.  The only circumstance in which the subject can be missing is when the observation is made by a device that does not know the patient. In this case, the observation SHALL be matched to a patient through some context/channel matching technique, and at this point, the observation should be updated. -If the target of the observation is different than the subject, the general extension [observation-focal-subject](http://hl7.org/fhir/STU3/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
+If the target of the observation is different than the subject, the general extension [observation-focal-subject](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
@@ -713,7 +713,7 @@
     <t>Normally, an observation will have either a single value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and related observations (for an Apgar score, the observations from which the measure is derived). If a value is present, the datatype for this element should be determined by Observation.code. This element has a variable name depending on the type as follows: valueQuantity, valueCodeableConcept, valueString, valueBoolean, valueRange, valueRatio, valueSampledData, valueAttachment, valueTime, valueDateTime, or valuePeriod. (The name format is "'value' + the type name" with a capital on the first letter of the type).  -If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
@@ -840,7 +840,7 @@
     <t>Indicates the site on the subject's body where the observation was made (i.e. the target site).</t>
   </si>
   <si>
-    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](http://hl7.org/fhir/STU3/extension-body-site-instance.html).</t>
+    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-body-site-instance.html).</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1139,7 +1139,7 @@
     <t>A  reference to another resource (usually another Observation) whose relationship is defined by the relationship type code.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](http://hl7.org/fhir/STU3/observation.html#4.20.4).</t>
+    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#4.20.4).</t>
   </si>
   <si>
     <t>Normally, an observation will have either a value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and a set of related observations or sometimes a QuestionnaireResponse from which the measure is derived.</t>
@@ -1198,7 +1198,7 @@
     <t>Resource that is related to this one</t>
   </si>
   <si>
-    <t>A reference to the observation or [QuestionnaireResponse](http://hl7.org/fhir/STU3/questionnaireresponse.html#) resource that is related to this observation.</t>
+    <t>A reference to the observation or [QuestionnaireResponse](https://build.fhir.org/ig/hl7au/au-fhir-base/questionnaireresponse.html#) resource that is related to this observation.</t>
   </si>
   <si>
     <t>.targetObservation</t>
@@ -1213,7 +1213,7 @@
     <t>Some observations have multiple component observations.  These component observations are expressed as separate code value pairs that share the same attributes.  Examples include systolic and diastolic component observations for blood pressure measurement and multiple component observations for genetics observations.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>Component observations share the same attributes in the Observation resource as the primary observation and are always treated a part of a single observation (they are not separable).   However, the reference range for the primary observation value is not inherited by the component values and is required when appropriate for each component observation.</t>

</xml_diff>

<commit_message>
Regenerated SHS FHIR IG with updated Composition profile to include constraints on elements with Reference, relative FHIRPaths and use patternCodeableConcept to fix values of CodeableConcept elements; Fixes #62, Fixes #69, Fixes #54
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
+++ b/output/SharedHealthSummary/observation-norelevantfinding-1.xlsx
@@ -701,9 +701,6 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -719,9 +716,6 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">type:$this}
 </t>
   </si>
@@ -748,7 +742,13 @@
     <t>363714003 |Interprets|</t>
   </si>
   <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
     <t>Coded value of the observation</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -3849,9 +3849,7 @@
       <c r="A21" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="B21" t="s" s="2">
-        <v>217</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
@@ -3863,7 +3861,7 @@
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3875,16 +3873,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3909,24 +3907,26 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y21" t="s" s="2">
-        <v>222</v>
+        <v>45</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AE21" t="s" s="2">
         <v>216</v>
@@ -3938,36 +3938,36 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK21" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM21" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>230</v>
-      </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>216</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>45</v>
@@ -3980,7 +3980,7 @@
         <v>56</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
@@ -3992,16 +3992,16 @@
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L22" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4026,11 +4026,11 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4057,28 +4057,28 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO22" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>230</v>
       </c>
     </row>
     <row r="23" hidden="true">
@@ -4182,7 +4182,7 @@
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
@@ -7390,13 +7390,13 @@
         <v>395</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>396</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7466,16 +7466,16 @@
         <v>397</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO51" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>230</v>
       </c>
     </row>
     <row r="52" hidden="true">

</xml_diff>